<commit_message>
updates show table and all
</commit_message>
<xml_diff>
--- a/attachments/correctExcel.xlsx
+++ b/attachments/correctExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/Fina-Health/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F8039E-803D-5C41-8B9F-E0E4F26CE3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF66B9BA-0D49-8B43-8D24-DE2210D25693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="4420" windowWidth="23260" windowHeight="12460" xr2:uid="{B00E6A59-B660-44BB-BDEB-6009DE29DE37}"/>
+    <workbookView xWindow="5540" yWindow="1580" windowWidth="23260" windowHeight="12460" xr2:uid="{B00E6A59-B660-44BB-BDEB-6009DE29DE37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Batch id:</t>
   </si>
   <si>
-    <t>BI124</t>
-  </si>
-  <si>
     <t>delivery date:</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t xml:space="preserve">Surgical_mask </t>
   </si>
   <si>
-    <t xml:space="preserve">Thermometer </t>
-  </si>
-  <si>
     <t xml:space="preserve">Surgical_gown </t>
   </si>
   <si>
@@ -82,13 +76,13 @@
     <t xml:space="preserve">Plaster </t>
   </si>
   <si>
-    <t xml:space="preserve">Needle </t>
-  </si>
-  <si>
     <t xml:space="preserve">Gloove </t>
   </si>
   <si>
     <t xml:space="preserve">Cottons </t>
+  </si>
+  <si>
+    <t>BIE24</t>
   </si>
 </sst>
 </file>
@@ -453,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E16A14-FD1C-4A22-85D2-CF09AFF87255}">
-  <dimension ref="A4:D18"/>
+  <dimension ref="A4:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -471,15 +465,15 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -487,16 +481,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -504,13 +498,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -518,13 +512,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3">
         <v>6</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -532,13 +526,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -546,13 +540,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -560,13 +554,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="3">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -574,13 +568,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -591,45 +585,17 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="C15">
-        <v>16</v>
-      </c>
-      <c r="D15">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="B16" s="4">
         <v>1235</v>
       </c>
     </row>

</xml_diff>